<commit_message>
added sample images, rewritten the ReadMe
</commit_message>
<xml_diff>
--- a/cdp.xlsx
+++ b/cdp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182BD60C-70BE-4402-B48E-57405799E5E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6984853B-A173-47B5-929C-E0D058271790}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,15 +453,15 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -471,6 +471,9 @@
   <dxfs count="4">
     <dxf>
       <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -491,9 +494,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -516,7 +516,7 @@
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Iteration"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Node title"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tree path"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Depth" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Depth" dataDxfId="1">
       <calculatedColumnFormula>IF(E3="","",LEN(E3)-LEN(SUBSTITUTE(E3,"/",""))+1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Resource type"/>
@@ -854,7 +854,7 @@
   <dimension ref="B2:W649"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,7 +865,7 @@
     <col min="5" max="5" width="48.5546875" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -888,7 +888,7 @@
       <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I2" t="s">
@@ -897,7 +897,7 @@
       <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>117</v>
       </c>
       <c r="W2" t="s">
@@ -921,7 +921,7 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J3" t="b">
@@ -952,7 +952,7 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I4" t="s">
@@ -986,7 +986,7 @@
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="b">
@@ -1017,7 +1017,7 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J6" t="b">
@@ -1048,7 +1048,7 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J7" t="b">
@@ -1079,7 +1079,7 @@
       <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="J8" t="b">
@@ -1110,7 +1110,7 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="J9" t="b">
@@ -1138,7 +1138,7 @@
       <c r="G10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="J10" t="b">
@@ -1163,7 +1163,7 @@
       <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J11" t="b">
@@ -1188,7 +1188,7 @@
       <c r="G12" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J12" t="b">
@@ -1213,7 +1213,7 @@
       <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J13" t="b">
@@ -1238,7 +1238,7 @@
       <c r="G14" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J14" t="b">
@@ -1263,7 +1263,7 @@
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J15" t="b">
@@ -1288,7 +1288,7 @@
       <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J16" t="b">
@@ -1313,7 +1313,7 @@
       <c r="G17" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>51</v>
       </c>
       <c r="J17" t="b">
@@ -1338,7 +1338,7 @@
       <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J18" t="b">
@@ -1363,7 +1363,7 @@
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>56</v>
       </c>
       <c r="J19" t="b">
@@ -1388,7 +1388,7 @@
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>58</v>
       </c>
       <c r="J20" t="b">
@@ -1413,7 +1413,7 @@
       <c r="G21" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="J21" t="b">
@@ -1438,7 +1438,7 @@
       <c r="G22" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>63</v>
       </c>
       <c r="J22" t="b">
@@ -1463,7 +1463,7 @@
       <c r="G23" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="J23" t="b">
@@ -1488,7 +1488,7 @@
       <c r="G24" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>68</v>
       </c>
       <c r="J24" t="b">
@@ -1513,7 +1513,7 @@
       <c r="G25" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>71</v>
       </c>
       <c r="J25" t="b">
@@ -1538,7 +1538,7 @@
       <c r="G26" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J26" t="b">
@@ -1563,7 +1563,7 @@
       <c r="G27" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="3" t="s">
         <v>78</v>
       </c>
       <c r="J27" t="b">
@@ -1588,7 +1588,7 @@
       <c r="G28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J28" t="b">
@@ -1613,7 +1613,7 @@
       <c r="G29" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>77</v>
       </c>
       <c r="J29" t="b">
@@ -1638,7 +1638,7 @@
       <c r="G30" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>81</v>
       </c>
       <c r="J30" t="b">
@@ -1663,7 +1663,7 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J31" t="b">
@@ -1688,7 +1688,7 @@
       <c r="G32" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="3" t="s">
         <v>85</v>
       </c>
       <c r="J32" t="b">
@@ -1713,7 +1713,7 @@
       <c r="G33" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="3" t="s">
         <v>87</v>
       </c>
       <c r="J33" t="b">
@@ -1738,7 +1738,7 @@
       <c r="G34" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="3" t="s">
         <v>90</v>
       </c>
       <c r="J34" t="b">
@@ -1763,7 +1763,7 @@
       <c r="G35" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="3" t="s">
         <v>93</v>
       </c>
       <c r="J35" t="b">
@@ -1788,7 +1788,7 @@
       <c r="G36" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J36" t="b">
@@ -1813,7 +1813,7 @@
       <c r="G37" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="3" t="s">
         <v>99</v>
       </c>
       <c r="J37" t="b">
@@ -1838,7 +1838,7 @@
       <c r="G38" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="3" t="s">
         <v>101</v>
       </c>
       <c r="J38" t="b">
@@ -1863,7 +1863,7 @@
       <c r="G39" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="3" t="s">
         <v>103</v>
       </c>
       <c r="J39" t="b">
@@ -1888,7 +1888,7 @@
       <c r="G40" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="3" t="s">
         <v>106</v>
       </c>
       <c r="J40" t="b">
@@ -1913,7 +1913,7 @@
       <c r="G41" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="3" t="s">
         <v>109</v>
       </c>
       <c r="J41" t="b">
@@ -1938,7 +1938,7 @@
       <c r="G42" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="3" t="s">
         <v>112</v>
       </c>
       <c r="J42" t="b">
@@ -1963,7 +1963,7 @@
       <c r="G43" t="s">
         <v>10</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" s="3" t="s">
         <v>113</v>
       </c>
       <c r="J43" t="b">
@@ -1988,7 +1988,7 @@
       <c r="G44" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H44" s="3" t="s">
         <v>115</v>
       </c>
       <c r="J44" t="b">
@@ -2013,7 +2013,7 @@
       <c r="G45" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H45" s="3" t="s">
         <v>116</v>
       </c>
       <c r="J45" t="b">
@@ -6039,10 +6039,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3:J101">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
     <cfRule type="iconSet" priority="3">
@@ -6149,11 +6149,11 @@
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">

</xml_diff>